<commit_message>
Problem 37 Java Solution Backtracking 5.2% 92%
</commit_message>
<xml_diff>
--- a/Java/performance.xlsx
+++ b/Java/performance.xlsx
@@ -19,9 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Backtracking</t>
+  </si>
+  <si>
+    <t>95.5%-100%</t>
   </si>
 </sst>
 </file>
@@ -830,14 +833,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A17:C17"/>
+  <dimension ref="A17:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -852,6 +857,28 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.88749999999999996</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="C37" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Problem 39 Java Backtracking 100% 71%
</commit_message>
<xml_diff>
--- a/Java/performance.xlsx
+++ b/Java/performance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="2">
   <si>
     <t>Backtracking</t>
   </si>
@@ -833,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A17:C37"/>
+  <dimension ref="A17:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,6 +879,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>1</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="C39" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Problem 50 Java Solution Backtracking 66.45% 91%
</commit_message>
<xml_diff>
--- a/Java/performance.xlsx
+++ b/Java/performance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
   <si>
     <t>Backtracking</t>
   </si>
@@ -833,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A17:C39"/>
+  <dimension ref="A17:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -890,6 +890,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.91</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Problem 1512 and 2469 100% Solution
</commit_message>
<xml_diff>
--- a/Java/performance.xlsx
+++ b/Java/performance.xlsx
@@ -19,12 +19,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
   <si>
     <t>Backtracking</t>
   </si>
   <si>
     <t>95.5%-100%</t>
+  </si>
+  <si>
+    <t>Math</t>
+  </si>
+  <si>
+    <t>Hashmap</t>
   </si>
 </sst>
 </file>
@@ -833,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A17:C40"/>
+  <dimension ref="A17:D2739"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A1509" workbookViewId="0">
+      <selection activeCell="A1512" sqref="A1512"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,6 +907,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="1512" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1512" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1512" s="2">
+        <v>0.35759999999999997</v>
+      </c>
+      <c r="C1512" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1512" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2739" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2739" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2739" s="2">
+        <v>0.83109999999999995</v>
+      </c>
+      <c r="C2739" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Problem 9 Updated Math 99.59 63.55
</commit_message>
<xml_diff>
--- a/Java/performance.xlsx
+++ b/Java/performance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
     <t>Backtracking</t>
   </si>
@@ -839,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A17:D2739"/>
+  <dimension ref="A9:D2739"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1509" workbookViewId="0">
-      <selection activeCell="A1512" sqref="A1512"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,6 +852,17 @@
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>0.99590000000000001</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.63549999999999995</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>

</xml_diff>